<commit_message>
update before meeting on march 16
</commit_message>
<xml_diff>
--- a/suitability/ecocrop_runs.xlsx
+++ b/suitability/ecocrop_runs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anibi\Documents\codes\WFP-profiles\suitability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C4485-1A55-4DE0-B2E2-DD2CDF00810F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7FCC9-94AD-4E42-9F26-73CEEB9B67C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{38876EFD-73BB-403A-8494-D93714BC772B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="299">
   <si>
     <t>NAME</t>
   </si>
@@ -881,13 +881,64 @@
   </si>
   <si>
     <t>"maize_all","peas","bean","cassava","ship/goat","poultry","cattle"</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>BDI</t>
+  </si>
+  <si>
+    <t>Plaine de l'Imbo</t>
+  </si>
+  <si>
+    <t>Depressions de l'est</t>
+  </si>
+  <si>
+    <t>Depressions du Nord</t>
+  </si>
+  <si>
+    <t>Plateaux secs de l'Est</t>
+  </si>
+  <si>
+    <t>"bean", "cassava", "maize_all"</t>
+  </si>
+  <si>
+    <t>"cassava", "bean", "maize_all"</t>
+  </si>
+  <si>
+    <t>"African_rice", "maize_all", "cassava"</t>
+  </si>
+  <si>
+    <t>"maize_all","African_rice","bean","cattle","ship/goat","poultry"</t>
+  </si>
+  <si>
+    <t>"bean", "sorghum_all", "cassava"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -910,6 +961,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -944,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,6 +1022,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1808,10 +1868,10 @@
   <dimension ref="A1:Q94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6488,7 +6548,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6522,7 +6582,7 @@
         <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
         <v>275</v>
@@ -6539,7 +6599,7 @@
         <v>271</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
         <v>276</v>
@@ -6556,7 +6616,7 @@
         <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C4" t="s">
         <v>277</v>
@@ -6573,7 +6633,7 @@
         <v>271</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
         <v>278</v>
@@ -6583,6 +6643,125 @@
       </c>
       <c r="E5" s="3" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D12" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>